<commit_message>
First UI example (broken chart)
</commit_message>
<xml_diff>
--- a/data/measurements.xlsx
+++ b/data/measurements.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\core-time-distribution\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{45845F75-1D40-44BC-9DAF-515F1D94025A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4703C35E-0B4F-486C-8DC1-E79C5D153C9E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="945" yWindow="0" windowWidth="27855" windowHeight="12810" xr2:uid="{383D0F8A-80DE-4183-AA79-998C9EBB31A5}"/>
+    <workbookView xWindow="2835" yWindow="0" windowWidth="27855" windowHeight="12810" xr2:uid="{383D0F8A-80DE-4183-AA79-998C9EBB31A5}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="data" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -24,16 +24,44 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Jonas Hörström</author>
+  </authors>
+  <commentList>
+    <comment ref="B16" authorId="0" shapeId="0" xr:uid="{2D7822FF-0C70-415B-9D73-5D29F21E5805}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Jonas Hörström:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Guess</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Date</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Size</t>
   </si>
   <si>
     <t>feature</t>
@@ -44,12 +72,18 @@
   <si>
     <t>admin</t>
   </si>
+  <si>
+    <t>maintenance</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,6 +105,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -98,8 +145,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,308 +461,416 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DE8ED03-4D3C-4947-B562-C11A10B99997}">
-  <dimension ref="A1:C26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F26DE08-26C9-4756-98F3-63C57DAC1B0B}">
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C40" sqref="C39:C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="14.85546875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>43584</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
+      <c r="B2" s="4">
+        <v>0.3</v>
       </c>
       <c r="C2" s="4">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>43584</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="4">
+      <c r="B3" s="4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E3" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>43584</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
+      <c r="B4" s="4">
+        <v>0</v>
       </c>
       <c r="C4" s="4">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E4" s="4">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>43584</v>
       </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
       <c r="C5" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>43584</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="4">
+        <v>43585</v>
+      </c>
+      <c r="B6" s="4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E6" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>43584</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
+        <v>43585</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.25</v>
       </c>
       <c r="C7" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>43585</v>
+      </c>
+      <c r="B8" s="4">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>43584</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="4">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E8" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>43585</v>
       </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
       <c r="C9" s="4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>43585</v>
       </c>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
       <c r="C10" s="4">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>43585</v>
-      </c>
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="4">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>43587</v>
+      </c>
+      <c r="B11" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>43585</v>
-      </c>
-      <c r="B12" t="s">
-        <v>4</v>
+        <v>43587</v>
       </c>
       <c r="C12" s="4">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>43585</v>
-      </c>
-      <c r="B13" t="s">
-        <v>4</v>
+        <v>43587</v>
       </c>
       <c r="C13" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>43585</v>
-      </c>
-      <c r="B14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>43588</v>
+      </c>
+      <c r="B14" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>43585</v>
-      </c>
-      <c r="B15" t="s">
-        <v>5</v>
+        <v>43588</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0.15</v>
       </c>
       <c r="C15" s="4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>43585</v>
-      </c>
-      <c r="B16" t="s">
-        <v>5</v>
+        <v>43588</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0.15</v>
       </c>
       <c r="C16" s="4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>43585</v>
-      </c>
-      <c r="B17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>43591</v>
+      </c>
+      <c r="B17" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>43585</v>
-      </c>
-      <c r="B18" t="s">
-        <v>5</v>
+        <v>43591</v>
       </c>
       <c r="C18" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>43591</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>43592</v>
+      </c>
+      <c r="B20" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>43592</v>
+      </c>
+      <c r="B21" s="4">
+        <v>0.875</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>43592</v>
+      </c>
+      <c r="B22" s="4">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>43587</v>
-      </c>
-      <c r="B19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>43587</v>
-      </c>
-      <c r="B20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>43587</v>
-      </c>
-      <c r="B21" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>43588</v>
-      </c>
-      <c r="B22" t="s">
-        <v>3</v>
-      </c>
       <c r="C22" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.6</v>
+      </c>
+      <c r="E22" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>43588</v>
-      </c>
-      <c r="B23" t="s">
-        <v>3</v>
+        <v>43592</v>
+      </c>
+      <c r="B23" s="4">
+        <v>0.3</v>
       </c>
       <c r="C23" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="E23" s="4">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>43592</v>
+      </c>
+      <c r="D24" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="E24" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>43593</v>
+      </c>
+      <c r="B25" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="E25" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>43593</v>
+      </c>
+      <c r="B26" s="4">
+        <v>0.875</v>
+      </c>
+      <c r="E26" s="4">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>43593</v>
+      </c>
+      <c r="C27" s="4">
+        <v>0.875</v>
+      </c>
+      <c r="E27" s="4">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>43593</v>
+      </c>
+      <c r="C28" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="D28" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="E28" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>43593</v>
+      </c>
+      <c r="D29" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="E29" s="4">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>43594</v>
+      </c>
+      <c r="B30" s="4">
+        <v>0.875</v>
+      </c>
+      <c r="E30" s="4">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>43594</v>
+      </c>
+      <c r="B31" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="D31" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="E31" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>43594</v>
+      </c>
+      <c r="B32" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="C32" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="E32" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>43594</v>
+      </c>
+      <c r="C33" s="4">
+        <v>0.875</v>
+      </c>
+      <c r="E33" s="4">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>43595</v>
+      </c>
+      <c r="B34" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="E34" s="4">
         <v>0.15</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <v>43588</v>
-      </c>
-      <c r="B24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="4">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>43595</v>
+      </c>
+      <c r="C35" s="4">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>43588</v>
-      </c>
-      <c r="B25" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="4">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>43588</v>
-      </c>
-      <c r="B26" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="4">
+      <c r="E35" s="4">
         <v>0.15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding selections to the chart
</commit_message>
<xml_diff>
--- a/data/measurements.xlsx
+++ b/data/measurements.xlsx
@@ -1,24 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\core-time-distribution\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bgk/git/core-time-distribution/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{86BC772A-8FAC-4E3C-8918-4C818C55DA29}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BB686B-0476-6243-8928-2A911952B00B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="0" windowWidth="27855" windowHeight="12810" xr2:uid="{383D0F8A-80DE-4183-AA79-998C9EBB31A5}"/>
+    <workbookView xWindow="5880" yWindow="-27400" windowWidth="14200" windowHeight="20860" xr2:uid="{383D0F8A-80DE-4183-AA79-998C9EBB31A5}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -59,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -74,6 +80,9 @@
   </si>
   <si>
     <t>maintenance</t>
+  </si>
+  <si>
+    <t>entryconrtrol</t>
   </si>
 </sst>
 </file>
@@ -141,12 +150,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,19 +473,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F26DE08-26C9-4756-98F3-63C57DAC1B0B}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="5" width="14.85546875" style="4" customWidth="1"/>
+    <col min="2" max="5" width="14.83203125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -490,8 +501,11 @@
       <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>43584</v>
       </c>
@@ -507,8 +521,12 @@
       <c r="E2" s="4">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="5">
+        <f>SUM(B2:E2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>43584</v>
       </c>
@@ -518,8 +536,12 @@
       <c r="E3" s="4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="5">
+        <f t="shared" ref="F3:F60" si="0">SUM(B3:E3)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>43584</v>
       </c>
@@ -532,16 +554,24 @@
       <c r="E4" s="4">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>43584</v>
       </c>
       <c r="C5" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>43585</v>
       </c>
@@ -551,8 +581,12 @@
       <c r="E6" s="4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>43585</v>
       </c>
@@ -565,8 +599,12 @@
       <c r="E7" s="4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>43585</v>
       </c>
@@ -576,16 +614,24 @@
       <c r="E8" s="4">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>43585</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>43585</v>
       </c>
@@ -595,40 +641,60 @@
       <c r="E10" s="4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>43587</v>
       </c>
       <c r="B11" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>43587</v>
       </c>
       <c r="C12" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>43587</v>
       </c>
       <c r="C13" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>43588</v>
       </c>
       <c r="B14" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>43588</v>
       </c>
@@ -638,8 +704,12 @@
       <c r="C15" s="4">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>43588</v>
       </c>
@@ -649,8 +719,12 @@
       <c r="C16" s="4">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>43591</v>
       </c>
@@ -660,16 +734,24 @@
       <c r="E17" s="4">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>43591</v>
       </c>
       <c r="C18" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>43591</v>
       </c>
@@ -679,16 +761,24 @@
       <c r="E19" s="4">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>43592</v>
       </c>
       <c r="B20" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>43592</v>
       </c>
@@ -698,8 +788,12 @@
       <c r="E21" s="4">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>43592</v>
       </c>
@@ -712,8 +806,12 @@
       <c r="E22" s="4">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="5">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>43592</v>
       </c>
@@ -726,8 +824,12 @@
       <c r="E23" s="4">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>43592</v>
       </c>
@@ -737,8 +839,12 @@
       <c r="E24" s="4">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>43593</v>
       </c>
@@ -748,8 +854,12 @@
       <c r="E25" s="4">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>43593</v>
       </c>
@@ -759,8 +869,12 @@
       <c r="E26" s="4">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>43593</v>
       </c>
@@ -770,8 +884,12 @@
       <c r="E27" s="4">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>43593</v>
       </c>
@@ -784,8 +902,12 @@
       <c r="E28" s="4">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>43593</v>
       </c>
@@ -795,8 +917,12 @@
       <c r="E29" s="4">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>43594</v>
       </c>
@@ -806,8 +932,12 @@
       <c r="E30" s="4">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>43594</v>
       </c>
@@ -820,8 +950,12 @@
       <c r="E31" s="4">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>43594</v>
       </c>
@@ -834,8 +968,12 @@
       <c r="E32" s="4">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>43594</v>
       </c>
@@ -845,8 +983,12 @@
       <c r="E33" s="4">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>43595</v>
       </c>
@@ -856,8 +998,12 @@
       <c r="E34" s="4">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>43595</v>
       </c>
@@ -867,8 +1013,12 @@
       <c r="E35" s="4">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>43595</v>
       </c>
@@ -880,11 +1030,378 @@
       </c>
       <c r="E36" s="4">
         <v>0.15</v>
+      </c>
+      <c r="F36" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
+        <v>43598</v>
+      </c>
+      <c r="B37" s="4">
+        <v>0.875</v>
+      </c>
+      <c r="E37" s="4">
+        <v>0.125</v>
+      </c>
+      <c r="F37" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="2">
+        <v>43598</v>
+      </c>
+      <c r="C38" s="4">
+        <v>0.875</v>
+      </c>
+      <c r="E38" s="4">
+        <v>0.125</v>
+      </c>
+      <c r="F38" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="2">
+        <v>43598</v>
+      </c>
+      <c r="C39" s="4">
+        <v>0.875</v>
+      </c>
+      <c r="E39" s="4">
+        <v>0.125</v>
+      </c>
+      <c r="F39" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="2">
+        <v>43598</v>
+      </c>
+      <c r="C40" s="4">
+        <v>0.875</v>
+      </c>
+      <c r="E40" s="4">
+        <v>0.125</v>
+      </c>
+      <c r="F40" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="2">
+        <v>43598</v>
+      </c>
+      <c r="D41" s="4">
+        <v>0.875</v>
+      </c>
+      <c r="E41" s="4">
+        <v>0.125</v>
+      </c>
+      <c r="F41" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="2">
+        <v>43599</v>
+      </c>
+      <c r="B42" s="4">
+        <v>0.875</v>
+      </c>
+      <c r="E42" s="4">
+        <v>0.125</v>
+      </c>
+      <c r="F42" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="2">
+        <v>43599</v>
+      </c>
+      <c r="B43" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="E43" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="F43" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="2">
+        <v>43599</v>
+      </c>
+      <c r="B44" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="D44" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="E44" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="F44" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="2">
+        <v>43599</v>
+      </c>
+      <c r="C45" s="4">
+        <v>0.625</v>
+      </c>
+      <c r="E45" s="4">
+        <v>0.375</v>
+      </c>
+      <c r="F45" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="2">
+        <v>43599</v>
+      </c>
+      <c r="D46" s="4">
+        <v>0.625</v>
+      </c>
+      <c r="E46" s="4">
+        <v>0.375</v>
+      </c>
+      <c r="F46" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="2">
+        <v>43599</v>
+      </c>
+      <c r="D47" s="4">
+        <v>0.625</v>
+      </c>
+      <c r="E47" s="4">
+        <v>0.375</v>
+      </c>
+      <c r="F47" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="2">
+        <v>43600</v>
+      </c>
+      <c r="B48" s="4">
+        <v>1</v>
+      </c>
+      <c r="F48" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="2">
+        <v>43600</v>
+      </c>
+      <c r="B49" s="4">
+        <v>1</v>
+      </c>
+      <c r="F49" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="2">
+        <v>43600</v>
+      </c>
+      <c r="B50" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="C50" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="E50" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="F50" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="2">
+        <v>43600</v>
+      </c>
+      <c r="D51" s="4">
+        <v>1</v>
+      </c>
+      <c r="F51" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="2">
+        <v>43600</v>
+      </c>
+      <c r="D52" s="4">
+        <v>1</v>
+      </c>
+      <c r="F52" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="2">
+        <v>43600</v>
+      </c>
+      <c r="D53" s="4">
+        <v>1</v>
+      </c>
+      <c r="F53" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="2">
+        <v>43601</v>
+      </c>
+      <c r="B54" s="4">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="D54" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="E54" s="4">
+        <v>0.125</v>
+      </c>
+      <c r="F54" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="2">
+        <v>43601</v>
+      </c>
+      <c r="B55" s="4">
+        <v>0.875</v>
+      </c>
+      <c r="E55" s="4">
+        <v>0.125</v>
+      </c>
+      <c r="F55" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="2">
+        <v>43601</v>
+      </c>
+      <c r="B56" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="D56" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="E56" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="F56" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="2">
+        <v>43601</v>
+      </c>
+      <c r="D57" s="4">
+        <v>1</v>
+      </c>
+      <c r="F57" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="2">
+        <v>43601</v>
+      </c>
+      <c r="D58" s="4">
+        <v>0.875</v>
+      </c>
+      <c r="E58" s="4">
+        <v>0.125</v>
+      </c>
+      <c r="F58" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="2">
+        <v>43602</v>
+      </c>
+      <c r="B59" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="E59" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="F59" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="2">
+        <v>43602</v>
+      </c>
+      <c r="B60" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="C60" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="D60" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="E60" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="F60" s="5">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999989</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="F31:F32" formulaRange="1"/>
+  </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>